<commit_message>
Updating latest xls work
</commit_message>
<xml_diff>
--- a/test-tools/memory_timeout_results/NODE_MEMORY_TIMEOUT.xlsx
+++ b/test-tools/memory_timeout_results/NODE_MEMORY_TIMEOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/memory_timeout_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8A5173-9835-4148-B07A-EB9A9B7BA3D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4623E35-B7E5-4841-8B89-35BF2A883751}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="4060" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{29D7C9B0-7FB0-4B41-823F-294962DF5F11}"/>
+    <workbookView xWindow="6400" yWindow="4060" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{29D7C9B0-7FB0-4B41-823F-294962DF5F11}"/>
   </bookViews>
   <sheets>
     <sheet name="NODE 128" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,7 @@
     <sheet name="Sheet4" sheetId="8" r:id="rId4"/>
     <sheet name="NODE 1024" sheetId="3" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'NODE 1024'!$G$2:$G$18</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'NODE 1024'!$L$2:$L$18</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'NODE 128'!$G$2:$G$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'NODE 512'!$G$2:$G$18</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'NODE 1024'!$G$2:$G$18</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'NODE 1024'!$L$2:$L$18</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'NODE 128'!$G$2:$G$18</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'NODE 512'!$G$2:$G$18</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -414,7 +404,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; mins&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,6 +501,746 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NODE 128'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NODE 128'!$K$3:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NODE 128'!$G$3:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.76</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.57</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.77</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.43</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E907-E54B-A82F-25C0E67FA011}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="380200816"/>
+        <c:axId val="757958416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="380200816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="757958416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="757958416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="380200816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NODE 512'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'NODE 512'!$G$3:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>20.58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.88</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.6500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF32-5B47-9866-B08280A55970}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="638614640"/>
+        <c:axId val="638636688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="638614640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="638636688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="638636688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="638614640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1227,6 +1957,596 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$B$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>MEAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MEDIAN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MIN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MAX</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>STDDEV</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-400E-8348-BB2A-C648E25592E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$B$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>MEAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MEDIAN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MIN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MAX</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>STDDEV</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9127600848603201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.467999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.541600000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-400E-8348-BB2A-C648E25592E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$B$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>MEAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MEDIAN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MIN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MAX</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>STDDEV</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.381764705882353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8258911829281645</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.283999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-400E-8348-BB2A-C648E25592E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$B$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>MEAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MEDIAN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MIN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MAX</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>STDDEV</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.2711764705882356</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3032369827156574</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5899999999999928</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.597999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.350000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-400E-8348-BB2A-C648E25592E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1302096544"/>
+        <c:axId val="1341839120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1302096544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1341839120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1341839120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1302096544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1267,7 +2587,1662 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1782,6 +4757,88 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB08288-CF55-1C4C-9368-AED3480CC676}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2381250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C31F08-7A6E-8143-B2CC-63C5A21C6850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -1811,6 +4868,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9295E099-AE1E-6044-8901-27E5C8B8D92B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2114,16 +5212,16 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K18"/>
+      <selection activeCell="K1" activeCellId="3" sqref="G3:G18 K3:K18 G1 K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +5256,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2193,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2228,7 +5326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2263,7 +5361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2298,7 +5396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2333,7 +5431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2368,7 +5466,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2403,7 +5501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +5536,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2473,7 +5571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2508,7 +5606,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2543,7 +5641,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +5676,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -2613,7 +5711,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2648,7 +5746,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2683,7 +5781,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2718,7 +5816,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2755,18 +5853,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94CBE35-C5C7-724B-A4DA-30A1FFAFE438}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" activeCellId="3" sqref="G3:G18 K3:K18 K1 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
@@ -2779,7 +5878,7 @@
     <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2814,7 +5913,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2849,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2884,7 +5983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2919,7 +6018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2954,7 +6053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2989,7 +6088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3024,7 +6123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3059,7 +6158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3094,7 +6193,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3129,7 +6228,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3163,8 +6262,12 @@
       <c r="K11">
         <v>45</v>
       </c>
+      <c r="L11">
+        <f>SUM(K2:K11)</f>
+        <v>225</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3198,8 +6301,12 @@
       <c r="K12">
         <v>50</v>
       </c>
+      <c r="L12">
+        <f>L11/60</f>
+        <v>3.75</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3234,7 +6341,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3269,7 +6376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -3304,7 +6411,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -3339,7 +6446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -3374,7 +6481,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3411,6 +6518,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3418,13 +6526,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286BE167-F431-2047-A109-3FB91E92F121}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27" thickTop="1" thickBot="1">
       <c r="B1" s="4" t="s">
         <v>115</v>
       </c>
@@ -3450,7 +6558,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="27" thickTop="1" thickBot="1">
       <c r="A2" s="4">
         <v>128</v>
       </c>
@@ -3487,7 +6595,7 @@
         <v>37.06</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="27" thickTop="1" thickBot="1">
       <c r="A3" s="4">
         <v>512</v>
       </c>
@@ -3524,7 +6632,7 @@
         <v>20.58</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="27" thickTop="1" thickBot="1">
       <c r="A4" s="4">
         <v>1024</v>
       </c>
@@ -3561,9 +6669,10 @@
         <v>18.350000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:9" ht="17" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3575,7 +6684,7 @@
       <selection activeCell="G1" sqref="G1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
@@ -3588,7 +6697,7 @@
     <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +6732,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3662,7 +6771,7 @@
         <v>0 mins</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3701,7 +6810,7 @@
         <v>5 mins</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3740,7 +6849,7 @@
         <v>10 mins</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3779,7 +6888,7 @@
         <v>15 mins</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3818,7 +6927,7 @@
         <v>20 mins</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3857,7 +6966,7 @@
         <v>25 mins</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3896,7 +7005,7 @@
         <v>30 mins</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3935,7 +7044,7 @@
         <v>35 mins</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3974,7 +7083,7 @@
         <v>40 mins</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -4013,7 +7122,7 @@
         <v>45 mins</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4052,7 +7161,7 @@
         <v>50 mins</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4091,7 +7200,7 @@
         <v>55 mins</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -4130,7 +7239,7 @@
         <v>60 mins</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -4169,7 +7278,7 @@
         <v>65 mins</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -4208,7 +7317,7 @@
         <v>70 mins</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -4247,7 +7356,7 @@
         <v>75 mins</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>8</v>
       </c>

</xml_diff>